<commit_message>
Fausey Py and Conditions
</commit_message>
<xml_diff>
--- a/Stimulus set samples/Arnold Clue_stimuli.xlsx
+++ b/Stimulus set samples/Arnold Clue_stimuli.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Desktop/MakeMetasforStims/Stimulus set samples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="1860" windowWidth="32980" windowHeight="24660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List A" sheetId="1" r:id="rId1"/>
     <sheet name="List B" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -447,6 +455,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -778,9 +791,9 @@
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -836,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -872,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -893,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -929,7 +942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -950,7 +963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -986,7 +999,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1007,7 +1020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1028,7 +1041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1064,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1085,7 +1098,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1120,7 +1133,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1141,7 +1154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1176,7 +1189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1197,7 +1210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1232,7 +1245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1253,7 +1266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1288,7 +1301,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1309,7 +1322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1330,7 +1343,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1366,7 +1379,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1387,7 +1400,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1408,7 +1421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1444,7 +1457,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1465,7 +1478,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1500,7 +1513,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1521,7 +1534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1556,7 +1569,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1577,7 +1590,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1612,7 +1625,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1633,7 +1646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1668,7 +1681,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1689,7 +1702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1724,7 +1737,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1781,7 +1794,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1802,7 +1815,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1838,7 +1851,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1859,7 +1872,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1895,7 +1908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1916,7 +1929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1951,7 +1964,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1972,7 +1985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1993,7 +2006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2028,7 +2041,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2049,7 +2062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2085,7 +2098,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2106,7 +2119,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2142,7 +2155,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2163,7 +2176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2198,7 +2211,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2219,7 +2232,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2255,7 +2268,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2279,11 +2292,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2295,9 +2303,9 @@
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2326,7 +2334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2343,7 +2351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2372,7 +2380,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2389,7 +2397,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2418,7 +2426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2435,7 +2443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2464,7 +2472,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2481,7 +2489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2498,7 +2506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2527,7 +2535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2544,7 +2552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2573,7 +2581,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2590,7 +2598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2619,7 +2627,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2636,7 +2644,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2665,7 +2673,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2682,7 +2690,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2711,7 +2719,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2728,7 +2736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2745,7 +2753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2791,7 +2799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2808,7 +2816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2883,7 +2891,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2900,7 +2908,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2929,7 +2937,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2975,7 +2983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2992,7 +3000,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -3021,7 +3029,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -3067,7 +3075,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3084,7 +3092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -3113,7 +3121,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3130,7 +3138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -3159,7 +3167,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3176,7 +3184,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -3205,7 +3213,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3222,7 +3230,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -3251,7 +3259,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3268,7 +3276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3285,7 +3293,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -3314,7 +3322,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3331,7 +3339,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -3360,7 +3368,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3377,7 +3385,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -3406,7 +3414,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3423,7 +3431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -3452,7 +3460,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3469,7 +3477,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -3498,7 +3506,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3518,11 +3526,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3532,13 +3535,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>